<commit_message>
Updated BOMs and schematic for CC111X parts and io expander part
</commit_message>
<xml_diff>
--- a/HammamatsuBoardBOM.xlsx
+++ b/HammamatsuBoardBOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Quantity</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Supplier 1</t>
   </si>
   <si>
-    <t>Supplier Part Number 1</t>
-  </si>
-  <si>
     <t>Supplier 2</t>
   </si>
   <si>
@@ -55,15 +52,9 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>490-3458-6-ND</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>GRM1555C1H101JZ01D</t>
-  </si>
-  <si>
     <t>C_0402</t>
   </si>
   <si>
@@ -113,6 +104,36 @@
   </si>
   <si>
     <t>U1</t>
+  </si>
+  <si>
+    <t>311-1024-1-ND</t>
+  </si>
+  <si>
+    <t>CC0402JRNPO9BN101</t>
+  </si>
+  <si>
+    <t>Cut Tape</t>
+  </si>
+  <si>
+    <t>DigiReal</t>
+  </si>
+  <si>
+    <t>P10KJDKR-ND</t>
+  </si>
+  <si>
+    <t>311-1024-6-ND</t>
+  </si>
+  <si>
+    <t>Tape and Reel</t>
+  </si>
+  <si>
+    <t>311-1024-2-ND</t>
+  </si>
+  <si>
+    <t>P10KJTR-ND</t>
+  </si>
+  <si>
+    <t>3M9205DKR-ND</t>
   </si>
 </sst>
 </file>
@@ -148,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,17 +192,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,16 +516,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="39.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,154 +549,186 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>14</v>
+      <c r="K3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
+    <hyperlink ref="G4" r:id="rId2" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ103X/P10KJDKR-ND/577446"/>
+    <hyperlink ref="G2" r:id="rId3" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-6-ND/578920"/>
+    <hyperlink ref="F4" r:id="rId4" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ103X/P10KJTR-ND/146735"/>
+    <hyperlink ref="G3" r:id="rId5" display="http://www.digikey.com/product-detail/en/951210-4620-AR-PR/3M9205DKR-ND/1959678"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>